<commit_message>
Python TF tut + eerste planning
</commit_message>
<xml_diff>
--- a/Opdrachten.xlsx
+++ b/Opdrachten.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB220C48-29F7-4B2B-8710-551CB99A8374}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE29848-3D07-426C-8C6E-0B194ED84FCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1344" windowWidth="17280" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Verslag over implementatie NN op de devices</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Opmerking</t>
   </si>
   <si>
-    <t>2/3 papers gedaan</t>
-  </si>
-  <si>
     <t>Opdrachtomschrijving</t>
   </si>
   <si>
@@ -85,10 +82,16 @@
     <t>Raspberry Pi AI uitvoeren</t>
   </si>
   <si>
-    <t xml:space="preserve">Eerste planning opstelle </t>
-  </si>
-  <si>
-    <t>Opdrachtomschrijvingopstellen</t>
+    <t>Eerste planning opstellen</t>
+  </si>
+  <si>
+    <t>Opdrachtomschrijving opstellen</t>
+  </si>
+  <si>
+    <t>Pas na tutorial Tenserflow</t>
+  </si>
+  <si>
+    <t>predictionprobleem nog op te lossen</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,16 +512,16 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -526,15 +529,15 @@
         <v>43742</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -542,15 +545,18 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -558,7 +564,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -569,7 +575,7 @@
         <v>43751</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -580,7 +586,7 @@
         <v>43773</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -591,7 +597,7 @@
         <v>43582</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -602,7 +608,7 @@
         <v>43603</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -610,10 +616,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
19/12 lit studie update
</commit_message>
<xml_diff>
--- a/Opdrachten.xlsx
+++ b/Opdrachten.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90055FE1-2205-482E-AD72-DB3A3C321712}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B50FED-E009-477E-9811-4636417386A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1020" yWindow="8184" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Verslag over implementatie NN op de devices</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Implementatie NN op 1 device</t>
   </si>
   <si>
-    <t>Implementatie NN op 5devices</t>
-  </si>
-  <si>
     <t>Experimentele resultaten</t>
   </si>
   <si>
@@ -119,6 +117,60 @@
   </si>
   <si>
     <t>PPT verdediging af en oefenen</t>
+  </si>
+  <si>
+    <t>Opstellen algoritme</t>
+  </si>
+  <si>
+    <t>Opstellen dataverwerkingsalgoritme</t>
+  </si>
+  <si>
+    <t>Implementatie NN op 3 devices</t>
+  </si>
+  <si>
+    <t>Implementatie NN op 5 devices</t>
+  </si>
+  <si>
+    <t>situering cloud tov edge verhaal (niet lokaal)</t>
+  </si>
+  <si>
+    <t>bespreken ML algemeen</t>
+  </si>
+  <si>
+    <t>kadering NN binnen ML</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>sterktes, zwaktes van alle verschillende ML-technieken en waarom wij voor NN -&gt; nood aan low latency ( zie zelfrijdende auto's) kiezen</t>
+  </si>
+  <si>
+    <t>SBC's beschrijven + hoe lang nog ondersteund?</t>
+  </si>
+  <si>
+    <t>evolutie SBC</t>
+  </si>
+  <si>
+    <t>(CPU-RAM-kostprijs, algemene performantie, eventuele overzichtspaper)</t>
+  </si>
+  <si>
+    <t>benchmarking mbt machinelearning</t>
+  </si>
+  <si>
+    <t>mogelijke use-case uitwerken</t>
+  </si>
+  <si>
+    <t>state of the art</t>
+  </si>
+  <si>
+    <t>korte vermelding van deep learning</t>
+  </si>
+  <si>
+    <t>toep per MML techniek</t>
+  </si>
+  <si>
+    <t>types transferfuncties: rectifier en co</t>
   </si>
 </sst>
 </file>
@@ -187,7 +239,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
     <dxf>
@@ -484,13 +536,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{937167B6-15C3-4223-83C3-5194F0E68A12}" name="Opdrachten" displayName="Opdrachten" ref="A2:D33" totalsRowShown="0">
-  <autoFilter ref="A2:D33" xr:uid="{6756300F-EDE9-4CFE-8517-CD1DD5FA7400}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{937167B6-15C3-4223-83C3-5194F0E68A12}" name="Opdrachten" displayName="Opdrachten" ref="A2:E46" totalsRowShown="0">
+  <autoFilter ref="A2:E46" xr:uid="{6756300F-EDE9-4CFE-8517-CD1DD5FA7400}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AE4270C8-A833-4539-B292-AFA66296A3F9}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{0C04A14B-DD27-4D5B-A039-1828C31CF6C8}" name="Opdracht"/>
     <tableColumn id="3" xr3:uid="{3860BA8F-6775-419E-8F89-6B5472BB47D0}" name="Status"/>
     <tableColumn id="6" xr3:uid="{52548523-62B2-43C7-A3EC-DF948B61573C}" name="Opmerking"/>
+    <tableColumn id="4" xr3:uid="{818AEAAA-31BE-478D-9182-DD596664ACE4}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -759,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -788,6 +841,9 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
@@ -909,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14" s="3"/>
       <c r="H14" s="4"/>
@@ -919,33 +975,30 @@
         <v>43800</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
-        <v>43510</v>
+        <v>43813</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="3"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1">
-        <v>43525</v>
-      </c>
+    <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -953,88 +1006,255 @@
       <c r="F17" s="3"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1">
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
         <v>43556</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>43562</v>
+      </c>
+      <c r="B41" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1">
-        <v>43562</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>43582</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1">
-        <v>43582</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1">
-        <v>43589</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>43631</v>
+      </c>
+      <c r="B45" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1">
-        <v>43603</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1">
-        <v>43631</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>16</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B46" t="s">
         <v>15</v>
       </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1"/>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D16 D12 C3:D9 C20 D14 C10:C15 D23 C22:D22 C26 C24:D24">
+  <conditionalFormatting sqref="D19 D12 C3:D9 C42 D14 C10:C14 C44 C46 C15:D16 D17 D25:D27 C17:C37">
     <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1045,12 +1265,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D7 C20 C22 C26 C24 C5:C15">
+  <conditionalFormatting sqref="C4:D7 C42 C44 C46 C5:C37">
     <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Niet begonnen">
       <formula>NOT(ISERROR(SEARCH("Niet begonnen",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1061,12 +1281,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1077,12 +1297,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+  <conditionalFormatting sqref="C41">
     <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
     <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1093,12 +1313,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C40">
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
     <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1109,12 +1329,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="C39">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1125,12 +1345,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+  <conditionalFormatting sqref="C38">
     <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1141,12 +1361,12 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Bezig"</formula>
     </cfRule>
@@ -1157,9 +1377,9 @@
       <formula>"Klaar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+  <conditionalFormatting sqref="C45">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Niet begonnen">
-      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Niet begonnen",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>